<commit_message>
add configuration in quiz
</commit_message>
<xml_diff>
--- a/public/files/templates/template-import-soal.xlsx
+++ b/public/files/templates/template-import-soal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nooravipp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\Anaheim\rev_bmti\bmti-backend\public\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AEFB64-B5EA-4B51-9B22-9E6BE9FF9AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7167E0-285F-415F-A877-B8A07F0AD261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D7EC2A9E-C10A-4034-8858-568345F8F687}"/>
   </bookViews>
@@ -34,24 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Soal</t>
-  </si>
-  <si>
-    <t>Apakah nama ibu kota francis ?</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>Kuala Lumpur</t>
-  </si>
-  <si>
-    <t>Singapura</t>
-  </si>
-  <si>
-    <t>Paris</t>
   </si>
   <si>
     <t>pilihan A</t>
@@ -70,21 +55,6 @@
   </si>
   <si>
     <t>Note : pemilihan antra pilihan dan jawaban bersifat case sensitif</t>
-  </si>
-  <si>
-    <t>Nama lain dari karnivora adalah ?</t>
-  </si>
-  <si>
-    <t>Pemakan Tumbuhan</t>
-  </si>
-  <si>
-    <t>Pemakan Hewan</t>
-  </si>
-  <si>
-    <t>Pemakan Daging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pemakan Segalanya </t>
   </si>
 </sst>
 </file>
@@ -470,7 +440,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +455,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -493,60 +463,36 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>

</xml_diff>